<commit_message>
Added SMC Type 1,2,3 data
From SMC Plantation Yield Calculator
</commit_message>
<xml_diff>
--- a/ORGANON_yield_analysis/Douglas-fir Yield Tables and Permanent Plots.xlsx
+++ b/ORGANON_yield_analysis/Douglas-fir Yield Tables and Permanent Plots.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1258" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="61">
   <si>
     <t>Source</t>
   </si>
@@ -205,6 +205,12 @@
   <si>
     <t>Type I, II</t>
   </si>
+  <si>
+    <t>i+ii</t>
+  </si>
+  <si>
+    <t>i+ii+iii</t>
+  </si>
 </sst>
 </file>
 
@@ -214,7 +220,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,14 +229,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -259,7 +257,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -267,9 +265,6 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -589,11 +584,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M517"/>
+  <dimension ref="A1:M560"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A504" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A516" sqref="A516:XFD516"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16215,7 +16210,7 @@
         <v>36</v>
       </c>
       <c r="C432" t="str">
-        <f t="shared" ref="C432:C495" si="15">IF(ISBLANK(B432),A432,A432&amp;"_"&amp;B432)&amp;IF(ISBLANK(D432),"_SI50_"&amp;E432,"_SI100_"&amp;D432)</f>
+        <f t="shared" ref="C432:C494" si="15">IF(ISBLANK(B432),A432,A432&amp;"_"&amp;B432)&amp;IF(ISBLANK(D432),"_SI50_"&amp;E432,"_SI100_"&amp;D432)</f>
         <v>Curtis_et_al_1982_planted_SI50_85</v>
       </c>
       <c r="E432" s="3">
@@ -18320,31 +18315,48 @@
       <c r="A489" t="s">
         <v>50</v>
       </c>
+      <c r="B489" t="s">
+        <v>59</v>
+      </c>
       <c r="C489" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
-      </c>
-      <c r="E489" s="3">
+        <v>SMC_2016_i+ii_SI50_106</v>
+      </c>
+      <c r="E489">
         <v>106</v>
       </c>
       <c r="F489" s="3">
         <v>3</v>
       </c>
-      <c r="G489" s="6"/>
-      <c r="H489" s="6"/>
-      <c r="I489" s="6"/>
-      <c r="J489" s="6"/>
-      <c r="K489" s="6"/>
-      <c r="L489" s="6"/>
-      <c r="M489" s="6"/>
+      <c r="G489" s="6">
+        <v>8</v>
+      </c>
+      <c r="H489" s="6">
+        <v>933</v>
+      </c>
+      <c r="I489" s="6">
+        <v>947</v>
+      </c>
+      <c r="K489" s="6">
+        <v>57</v>
+      </c>
+      <c r="L489" s="6">
+        <v>370</v>
+      </c>
+      <c r="M489" s="6">
+        <v>4</v>
+      </c>
     </row>
     <row r="490" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A490" t="s">
         <v>50</v>
       </c>
+      <c r="B490" t="s">
+        <v>59</v>
+      </c>
       <c r="C490" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E490">
         <v>106</v>
@@ -18352,32 +18364,35 @@
       <c r="F490" s="3">
         <v>3</v>
       </c>
-      <c r="G490" s="7">
-        <v>8</v>
-      </c>
-      <c r="H490" s="7">
-        <v>933</v>
-      </c>
-      <c r="I490" s="7">
-        <v>947</v>
-      </c>
-      <c r="K490" s="7">
-        <v>57</v>
-      </c>
-      <c r="L490" s="7">
+      <c r="G490" s="6">
+        <v>13</v>
+      </c>
+      <c r="H490" s="6">
+        <v>2512</v>
+      </c>
+      <c r="I490" s="6">
+        <v>4069</v>
+      </c>
+      <c r="K490" s="6">
+        <v>103</v>
+      </c>
+      <c r="L490" s="6">
         <v>370</v>
       </c>
-      <c r="M490" s="7">
-        <v>4</v>
+      <c r="M490" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="491" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A491" t="s">
         <v>50</v>
       </c>
+      <c r="B491" t="s">
+        <v>59</v>
+      </c>
       <c r="C491" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E491">
         <v>106</v>
@@ -18385,32 +18400,35 @@
       <c r="F491" s="3">
         <v>3</v>
       </c>
-      <c r="G491" s="7">
-        <v>13</v>
-      </c>
-      <c r="H491" s="7">
-        <v>2512</v>
-      </c>
-      <c r="I491" s="7">
-        <v>4069</v>
-      </c>
-      <c r="K491" s="7">
-        <v>103</v>
-      </c>
-      <c r="L491" s="7">
+      <c r="G491" s="6">
+        <v>18</v>
+      </c>
+      <c r="H491" s="6">
+        <v>4425</v>
+      </c>
+      <c r="I491" s="6">
+        <v>10345</v>
+      </c>
+      <c r="K491" s="6">
+        <v>149</v>
+      </c>
+      <c r="L491" s="6">
         <v>370</v>
       </c>
-      <c r="M491" s="7">
-        <v>5</v>
+      <c r="M491" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="492" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A492" t="s">
         <v>50</v>
       </c>
+      <c r="B492" t="s">
+        <v>59</v>
+      </c>
       <c r="C492" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E492">
         <v>106</v>
@@ -18418,32 +18436,35 @@
       <c r="F492" s="3">
         <v>3</v>
       </c>
-      <c r="G492" s="7">
-        <v>18</v>
-      </c>
-      <c r="H492" s="7">
-        <v>4425</v>
-      </c>
-      <c r="I492" s="7">
-        <v>10345</v>
-      </c>
-      <c r="K492" s="7">
-        <v>149</v>
-      </c>
-      <c r="L492" s="7">
+      <c r="G492" s="6">
+        <v>23</v>
+      </c>
+      <c r="H492" s="6">
+        <v>6180</v>
+      </c>
+      <c r="I492" s="6">
+        <v>19253</v>
+      </c>
+      <c r="K492" s="6">
+        <v>190</v>
+      </c>
+      <c r="L492" s="6">
         <v>370</v>
       </c>
-      <c r="M492" s="7">
-        <v>7</v>
+      <c r="M492" s="6">
+        <v>8</v>
       </c>
     </row>
     <row r="493" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A493" t="s">
         <v>50</v>
       </c>
+      <c r="B493" t="s">
+        <v>59</v>
+      </c>
       <c r="C493" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E493">
         <v>106</v>
@@ -18451,32 +18472,35 @@
       <c r="F493" s="3">
         <v>3</v>
       </c>
-      <c r="G493" s="7">
-        <v>23</v>
-      </c>
-      <c r="H493" s="7">
-        <v>6180</v>
-      </c>
-      <c r="I493" s="7">
-        <v>19253</v>
-      </c>
-      <c r="K493" s="7">
-        <v>190</v>
-      </c>
-      <c r="L493" s="7">
+      <c r="G493" s="6">
+        <v>28</v>
+      </c>
+      <c r="H493" s="6">
+        <v>7555</v>
+      </c>
+      <c r="I493" s="6">
+        <v>29409</v>
+      </c>
+      <c r="K493" s="6">
+        <v>224</v>
+      </c>
+      <c r="L493" s="6">
         <v>370</v>
       </c>
-      <c r="M493" s="7">
-        <v>8</v>
+      <c r="M493" s="6">
+        <v>10</v>
       </c>
     </row>
     <row r="494" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A494" t="s">
         <v>50</v>
       </c>
+      <c r="B494" t="s">
+        <v>59</v>
+      </c>
       <c r="C494" t="str">
         <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E494">
         <v>106</v>
@@ -18484,32 +18508,35 @@
       <c r="F494" s="3">
         <v>3</v>
       </c>
-      <c r="G494" s="7">
-        <v>28</v>
-      </c>
-      <c r="H494" s="7">
-        <v>7555</v>
-      </c>
-      <c r="I494" s="7">
-        <v>29409</v>
-      </c>
-      <c r="K494" s="7">
-        <v>224</v>
-      </c>
-      <c r="L494" s="7">
+      <c r="G494" s="6">
+        <v>33</v>
+      </c>
+      <c r="H494" s="6">
+        <v>8536</v>
+      </c>
+      <c r="I494" s="6">
+        <v>39436</v>
+      </c>
+      <c r="K494" s="6">
+        <v>250</v>
+      </c>
+      <c r="L494" s="6">
         <v>370</v>
       </c>
-      <c r="M494" s="7">
-        <v>10</v>
+      <c r="M494" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="495" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A495" t="s">
         <v>50</v>
       </c>
+      <c r="B495" t="s">
+        <v>59</v>
+      </c>
       <c r="C495" t="str">
-        <f t="shared" si="15"/>
-        <v>SMC_2016_SI50_106</v>
+        <f t="shared" ref="C495:C517" si="17">IF(ISBLANK(B495),A495,A495&amp;"_"&amp;B495)&amp;IF(ISBLANK(D495),"_SI50_"&amp;E495,"_SI100_"&amp;D495)</f>
+        <v>SMC_2016_i+ii_SI50_106</v>
       </c>
       <c r="E495">
         <v>106</v>
@@ -18517,65 +18544,71 @@
       <c r="F495" s="3">
         <v>3</v>
       </c>
-      <c r="G495" s="7">
-        <v>33</v>
-      </c>
-      <c r="H495" s="7">
-        <v>8536</v>
-      </c>
-      <c r="I495" s="7">
-        <v>39436</v>
-      </c>
-      <c r="K495" s="7">
-        <v>250</v>
-      </c>
-      <c r="L495" s="7">
-        <v>370</v>
-      </c>
-      <c r="M495" s="7">
-        <v>11</v>
+      <c r="G495" s="6">
+        <v>38</v>
+      </c>
+      <c r="H495" s="6">
+        <v>9197</v>
+      </c>
+      <c r="I495" s="6">
+        <v>48425</v>
+      </c>
+      <c r="K495" s="6">
+        <v>269</v>
+      </c>
+      <c r="L495" s="6">
+        <v>338</v>
+      </c>
+      <c r="M495" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="496" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A496" t="s">
         <v>50</v>
       </c>
+      <c r="B496" t="s">
+        <v>59</v>
+      </c>
       <c r="C496" t="str">
-        <f t="shared" ref="C496:C517" si="17">IF(ISBLANK(B496),A496,A496&amp;"_"&amp;B496)&amp;IF(ISBLANK(D496),"_SI50_"&amp;E496,"_SI100_"&amp;D496)</f>
-        <v>SMC_2016_SI50_106</v>
+        <f t="shared" si="17"/>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E496">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F496" s="3">
         <v>3</v>
       </c>
-      <c r="G496" s="7">
-        <v>38</v>
-      </c>
-      <c r="H496" s="7">
-        <v>9197</v>
-      </c>
-      <c r="I496" s="7">
-        <v>48425</v>
-      </c>
-      <c r="K496" s="7">
-        <v>269</v>
-      </c>
-      <c r="L496" s="7">
-        <v>338</v>
-      </c>
-      <c r="M496" s="7">
-        <v>12</v>
+      <c r="G496" s="6">
+        <v>8</v>
+      </c>
+      <c r="H496" s="6">
+        <v>1078</v>
+      </c>
+      <c r="I496" s="6">
+        <v>1182</v>
+      </c>
+      <c r="K496" s="6">
+        <v>63</v>
+      </c>
+      <c r="L496" s="6">
+        <v>370</v>
+      </c>
+      <c r="M496" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="497" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A497" t="s">
         <v>50</v>
       </c>
+      <c r="B497" t="s">
+        <v>59</v>
+      </c>
       <c r="C497" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E497">
         <v>110</v>
@@ -18583,32 +18616,35 @@
       <c r="F497" s="3">
         <v>3</v>
       </c>
-      <c r="G497" s="7">
-        <v>8</v>
-      </c>
-      <c r="H497" s="7">
-        <v>1078</v>
-      </c>
-      <c r="I497" s="7">
-        <v>1182</v>
-      </c>
-      <c r="K497" s="7">
-        <v>63</v>
-      </c>
-      <c r="L497" s="7">
+      <c r="G497" s="6">
+        <v>13</v>
+      </c>
+      <c r="H497" s="6">
+        <v>2791</v>
+      </c>
+      <c r="I497" s="6">
+        <v>4876</v>
+      </c>
+      <c r="K497" s="6">
+        <v>112</v>
+      </c>
+      <c r="L497" s="6">
         <v>370</v>
       </c>
-      <c r="M497" s="7">
-        <v>4</v>
+      <c r="M497" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="498" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A498" t="s">
         <v>50</v>
       </c>
+      <c r="B498" t="s">
+        <v>59</v>
+      </c>
       <c r="C498" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E498">
         <v>110</v>
@@ -18616,32 +18652,35 @@
       <c r="F498" s="3">
         <v>3</v>
       </c>
-      <c r="G498" s="7">
-        <v>13</v>
-      </c>
-      <c r="H498" s="7">
-        <v>2791</v>
-      </c>
-      <c r="I498" s="7">
-        <v>4876</v>
-      </c>
-      <c r="K498" s="7">
-        <v>112</v>
-      </c>
-      <c r="L498" s="7">
+      <c r="G498" s="6">
+        <v>18</v>
+      </c>
+      <c r="H498" s="6">
+        <v>4772</v>
+      </c>
+      <c r="I498" s="6">
+        <v>11974</v>
+      </c>
+      <c r="K498" s="6">
+        <v>160</v>
+      </c>
+      <c r="L498" s="6">
         <v>370</v>
       </c>
-      <c r="M498" s="7">
-        <v>6</v>
+      <c r="M498" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="499" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A499" t="s">
         <v>50</v>
       </c>
+      <c r="B499" t="s">
+        <v>59</v>
+      </c>
       <c r="C499" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E499">
         <v>110</v>
@@ -18649,32 +18688,35 @@
       <c r="F499" s="3">
         <v>3</v>
       </c>
-      <c r="G499" s="7">
-        <v>18</v>
-      </c>
-      <c r="H499" s="7">
-        <v>4772</v>
-      </c>
-      <c r="I499" s="7">
-        <v>11974</v>
-      </c>
-      <c r="K499" s="7">
-        <v>160</v>
-      </c>
-      <c r="L499" s="7">
+      <c r="G499" s="6">
+        <v>23</v>
+      </c>
+      <c r="H499" s="6">
+        <v>6520</v>
+      </c>
+      <c r="I499" s="6">
+        <v>21647</v>
+      </c>
+      <c r="K499" s="6">
+        <v>202</v>
+      </c>
+      <c r="L499" s="6">
         <v>370</v>
       </c>
-      <c r="M499" s="7">
-        <v>7</v>
+      <c r="M499" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="500" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A500" t="s">
         <v>50</v>
       </c>
+      <c r="B500" t="s">
+        <v>59</v>
+      </c>
       <c r="C500" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E500">
         <v>110</v>
@@ -18682,32 +18724,35 @@
       <c r="F500" s="3">
         <v>3</v>
       </c>
-      <c r="G500" s="7">
-        <v>23</v>
-      </c>
-      <c r="H500" s="7">
-        <v>6520</v>
-      </c>
-      <c r="I500" s="7">
-        <v>21647</v>
-      </c>
-      <c r="K500" s="7">
-        <v>202</v>
-      </c>
-      <c r="L500" s="7">
+      <c r="G500" s="6">
+        <v>28</v>
+      </c>
+      <c r="H500" s="6">
+        <v>7842</v>
+      </c>
+      <c r="I500" s="6">
+        <v>32281</v>
+      </c>
+      <c r="K500" s="6">
+        <v>235</v>
+      </c>
+      <c r="L500" s="6">
         <v>370</v>
       </c>
-      <c r="M500" s="7">
-        <v>9</v>
+      <c r="M500" s="6">
+        <v>10</v>
       </c>
     </row>
     <row r="501" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A501" t="s">
         <v>50</v>
       </c>
+      <c r="B501" t="s">
+        <v>59</v>
+      </c>
       <c r="C501" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E501">
         <v>110</v>
@@ -18715,32 +18760,35 @@
       <c r="F501" s="3">
         <v>3</v>
       </c>
-      <c r="G501" s="7">
-        <v>28</v>
-      </c>
-      <c r="H501" s="7">
-        <v>7842</v>
-      </c>
-      <c r="I501" s="7">
-        <v>32281</v>
-      </c>
-      <c r="K501" s="7">
-        <v>235</v>
-      </c>
-      <c r="L501" s="7">
-        <v>370</v>
-      </c>
-      <c r="M501" s="7">
-        <v>10</v>
+      <c r="G501" s="6">
+        <v>33</v>
+      </c>
+      <c r="H501" s="6">
+        <v>8758</v>
+      </c>
+      <c r="I501" s="6">
+        <v>42447</v>
+      </c>
+      <c r="K501" s="6">
+        <v>260</v>
+      </c>
+      <c r="L501" s="6">
+        <v>357</v>
+      </c>
+      <c r="M501" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="502" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A502" t="s">
         <v>50</v>
       </c>
+      <c r="B502" t="s">
+        <v>59</v>
+      </c>
       <c r="C502" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_110</v>
       </c>
       <c r="E502">
         <v>110</v>
@@ -18748,65 +18796,71 @@
       <c r="F502" s="3">
         <v>3</v>
       </c>
-      <c r="G502" s="7">
-        <v>33</v>
-      </c>
-      <c r="H502" s="7">
-        <v>8758</v>
-      </c>
-      <c r="I502" s="7">
-        <v>42447</v>
-      </c>
-      <c r="K502" s="7">
-        <v>260</v>
-      </c>
-      <c r="L502" s="7">
-        <v>357</v>
-      </c>
-      <c r="M502" s="7">
-        <v>12</v>
+      <c r="G502" s="6">
+        <v>38</v>
+      </c>
+      <c r="H502" s="6">
+        <v>9360</v>
+      </c>
+      <c r="I502" s="6">
+        <v>51300</v>
+      </c>
+      <c r="K502" s="6">
+        <v>279</v>
+      </c>
+      <c r="L502" s="6">
+        <v>314</v>
+      </c>
+      <c r="M502" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="503" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
         <v>50</v>
       </c>
+      <c r="B503" t="s">
+        <v>59</v>
+      </c>
       <c r="C503" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_110</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E503">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="F503" s="3">
-        <v>3</v>
-      </c>
-      <c r="G503" s="7">
-        <v>38</v>
-      </c>
-      <c r="H503" s="7">
-        <v>9360</v>
-      </c>
-      <c r="I503" s="7">
-        <v>51300</v>
-      </c>
-      <c r="K503" s="7">
-        <v>279</v>
-      </c>
-      <c r="L503" s="7">
-        <v>314</v>
-      </c>
-      <c r="M503" s="7">
-        <v>13</v>
+        <v>2</v>
+      </c>
+      <c r="G503" s="6">
+        <v>8</v>
+      </c>
+      <c r="H503" s="6">
+        <v>1288</v>
+      </c>
+      <c r="I503" s="6">
+        <v>1557</v>
+      </c>
+      <c r="K503" s="6">
+        <v>71</v>
+      </c>
+      <c r="L503" s="6">
+        <v>370</v>
+      </c>
+      <c r="M503" s="6">
+        <v>4</v>
       </c>
     </row>
     <row r="504" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A504" t="s">
         <v>50</v>
       </c>
+      <c r="B504" t="s">
+        <v>59</v>
+      </c>
       <c r="C504" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E504">
         <v>115</v>
@@ -18814,32 +18868,35 @@
       <c r="F504" s="3">
         <v>2</v>
       </c>
-      <c r="G504" s="7">
-        <v>8</v>
-      </c>
-      <c r="H504" s="7">
-        <v>1288</v>
-      </c>
-      <c r="I504" s="7">
-        <v>1557</v>
-      </c>
-      <c r="K504" s="7">
-        <v>71</v>
-      </c>
-      <c r="L504" s="7">
+      <c r="G504" s="6">
+        <v>13</v>
+      </c>
+      <c r="H504" s="6">
+        <v>3172</v>
+      </c>
+      <c r="I504" s="6">
+        <v>6089</v>
+      </c>
+      <c r="K504" s="6">
+        <v>124</v>
+      </c>
+      <c r="L504" s="6">
         <v>370</v>
       </c>
-      <c r="M504" s="7">
-        <v>4</v>
+      <c r="M504" s="6">
+        <v>6</v>
       </c>
     </row>
     <row r="505" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A505" t="s">
         <v>50</v>
       </c>
+      <c r="B505" t="s">
+        <v>59</v>
+      </c>
       <c r="C505" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E505">
         <v>115</v>
@@ -18847,32 +18904,35 @@
       <c r="F505" s="3">
         <v>2</v>
       </c>
-      <c r="G505" s="7">
-        <v>13</v>
-      </c>
-      <c r="H505" s="7">
-        <v>3172</v>
-      </c>
-      <c r="I505" s="7">
-        <v>6089</v>
-      </c>
-      <c r="K505" s="7">
-        <v>124</v>
-      </c>
-      <c r="L505" s="7">
+      <c r="G505" s="6">
+        <v>18</v>
+      </c>
+      <c r="H505" s="6">
+        <v>5223</v>
+      </c>
+      <c r="I505" s="6">
+        <v>14300</v>
+      </c>
+      <c r="K505" s="6">
+        <v>174</v>
+      </c>
+      <c r="L505" s="6">
         <v>370</v>
       </c>
-      <c r="M505" s="7">
-        <v>6</v>
+      <c r="M505" s="6">
+        <v>8</v>
       </c>
     </row>
     <row r="506" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A506" t="s">
         <v>50</v>
       </c>
+      <c r="B506" t="s">
+        <v>59</v>
+      </c>
       <c r="C506" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E506">
         <v>115</v>
@@ -18880,32 +18940,35 @@
       <c r="F506" s="3">
         <v>2</v>
       </c>
-      <c r="G506" s="7">
-        <v>18</v>
-      </c>
-      <c r="H506" s="7">
-        <v>5223</v>
-      </c>
-      <c r="I506" s="7">
-        <v>14300</v>
-      </c>
-      <c r="K506" s="7">
-        <v>174</v>
-      </c>
-      <c r="L506" s="7">
+      <c r="G506" s="6">
+        <v>23</v>
+      </c>
+      <c r="H506" s="6">
+        <v>6941</v>
+      </c>
+      <c r="I506" s="6">
+        <v>24915</v>
+      </c>
+      <c r="K506" s="6">
+        <v>216</v>
+      </c>
+      <c r="L506" s="6">
         <v>370</v>
       </c>
-      <c r="M506" s="7">
-        <v>8</v>
+      <c r="M506" s="6">
+        <v>9</v>
       </c>
     </row>
     <row r="507" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A507" t="s">
         <v>50</v>
       </c>
+      <c r="B507" t="s">
+        <v>59</v>
+      </c>
       <c r="C507" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E507">
         <v>115</v>
@@ -18913,32 +18976,35 @@
       <c r="F507" s="3">
         <v>2</v>
       </c>
-      <c r="G507" s="7">
-        <v>23</v>
-      </c>
-      <c r="H507" s="7">
-        <v>6941</v>
-      </c>
-      <c r="I507" s="7">
-        <v>24915</v>
-      </c>
-      <c r="K507" s="7">
-        <v>216</v>
-      </c>
-      <c r="L507" s="7">
+      <c r="G507" s="6">
+        <v>28</v>
+      </c>
+      <c r="H507" s="6">
+        <v>8186</v>
+      </c>
+      <c r="I507" s="6">
+        <v>36049</v>
+      </c>
+      <c r="K507" s="6">
+        <v>249</v>
+      </c>
+      <c r="L507" s="6">
         <v>370</v>
       </c>
-      <c r="M507" s="7">
-        <v>9</v>
+      <c r="M507" s="6">
+        <v>11</v>
       </c>
     </row>
     <row r="508" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A508" t="s">
         <v>50</v>
       </c>
+      <c r="B508" t="s">
+        <v>59</v>
+      </c>
       <c r="C508" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E508">
         <v>115</v>
@@ -18946,32 +19012,35 @@
       <c r="F508" s="3">
         <v>2</v>
       </c>
-      <c r="G508" s="7">
-        <v>28</v>
-      </c>
-      <c r="H508" s="7">
-        <v>8186</v>
-      </c>
-      <c r="I508" s="7">
-        <v>36049</v>
-      </c>
-      <c r="K508" s="7">
-        <v>249</v>
-      </c>
-      <c r="L508" s="7">
-        <v>370</v>
-      </c>
-      <c r="M508" s="7">
-        <v>11</v>
+      <c r="G508" s="6">
+        <v>33</v>
+      </c>
+      <c r="H508" s="6">
+        <v>9016</v>
+      </c>
+      <c r="I508" s="6">
+        <v>46259</v>
+      </c>
+      <c r="K508" s="6">
+        <v>274</v>
+      </c>
+      <c r="L508" s="6">
+        <v>325</v>
+      </c>
+      <c r="M508" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="509" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A509" t="s">
         <v>50</v>
       </c>
+      <c r="B509" t="s">
+        <v>59</v>
+      </c>
       <c r="C509" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_115</v>
       </c>
       <c r="E509">
         <v>115</v>
@@ -18979,65 +19048,71 @@
       <c r="F509" s="3">
         <v>2</v>
       </c>
-      <c r="G509" s="7">
-        <v>33</v>
-      </c>
-      <c r="H509" s="7">
-        <v>9016</v>
-      </c>
-      <c r="I509" s="7">
-        <v>46259</v>
-      </c>
-      <c r="K509" s="7">
-        <v>274</v>
-      </c>
-      <c r="L509" s="7">
-        <v>325</v>
-      </c>
-      <c r="M509" s="7">
-        <v>12</v>
+      <c r="G509" s="6">
+        <v>38</v>
+      </c>
+      <c r="H509" s="6">
+        <v>9544</v>
+      </c>
+      <c r="I509" s="6">
+        <v>54830</v>
+      </c>
+      <c r="K509" s="6">
+        <v>292</v>
+      </c>
+      <c r="L509" s="6">
+        <v>285</v>
+      </c>
+      <c r="M509" s="6">
+        <v>14</v>
       </c>
     </row>
     <row r="510" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A510" t="s">
         <v>50</v>
       </c>
+      <c r="B510" t="s">
+        <v>59</v>
+      </c>
       <c r="C510" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_115</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E510">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="F510" s="3">
         <v>2</v>
       </c>
-      <c r="G510" s="7">
-        <v>38</v>
-      </c>
-      <c r="H510" s="7">
-        <v>9544</v>
-      </c>
-      <c r="I510" s="7">
-        <v>54830</v>
-      </c>
-      <c r="K510" s="7">
-        <v>292</v>
-      </c>
-      <c r="L510" s="7">
-        <v>285</v>
-      </c>
-      <c r="M510" s="7">
-        <v>14</v>
+      <c r="G510" s="6">
+        <v>8</v>
+      </c>
+      <c r="H510" s="6">
+        <v>1515</v>
+      </c>
+      <c r="I510" s="6">
+        <v>2007</v>
+      </c>
+      <c r="K510" s="6">
+        <v>79</v>
+      </c>
+      <c r="L510" s="6">
+        <v>370</v>
+      </c>
+      <c r="M510" s="6">
+        <v>5</v>
       </c>
     </row>
     <row r="511" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A511" t="s">
         <v>50</v>
       </c>
+      <c r="B511" t="s">
+        <v>59</v>
+      </c>
       <c r="C511" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E511">
         <v>120</v>
@@ -19045,32 +19120,35 @@
       <c r="F511" s="3">
         <v>2</v>
       </c>
-      <c r="G511" s="7">
-        <v>8</v>
-      </c>
-      <c r="H511" s="7">
-        <v>1515</v>
-      </c>
-      <c r="I511" s="7">
-        <v>2007</v>
-      </c>
-      <c r="K511" s="7">
-        <v>79</v>
-      </c>
-      <c r="L511" s="7">
+      <c r="G511" s="6">
+        <v>13</v>
+      </c>
+      <c r="H511" s="6">
+        <v>3557</v>
+      </c>
+      <c r="I511" s="6">
+        <v>7456</v>
+      </c>
+      <c r="K511" s="6">
+        <v>136</v>
+      </c>
+      <c r="L511" s="6">
         <v>370</v>
       </c>
-      <c r="M511" s="7">
-        <v>5</v>
+      <c r="M511" s="6">
+        <v>7</v>
       </c>
     </row>
     <row r="512" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A512" t="s">
         <v>50</v>
       </c>
+      <c r="B512" t="s">
+        <v>59</v>
+      </c>
       <c r="C512" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E512">
         <v>120</v>
@@ -19078,32 +19156,35 @@
       <c r="F512" s="3">
         <v>2</v>
       </c>
-      <c r="G512" s="7">
-        <v>13</v>
-      </c>
-      <c r="H512" s="7">
-        <v>3557</v>
-      </c>
-      <c r="I512" s="7">
-        <v>7456</v>
-      </c>
-      <c r="K512" s="7">
-        <v>136</v>
-      </c>
-      <c r="L512" s="7">
+      <c r="G512" s="6">
+        <v>18</v>
+      </c>
+      <c r="H512" s="6">
+        <v>5654</v>
+      </c>
+      <c r="I512" s="6">
+        <v>16776</v>
+      </c>
+      <c r="K512" s="6">
+        <v>188</v>
+      </c>
+      <c r="L512" s="6">
         <v>370</v>
       </c>
-      <c r="M512" s="7">
-        <v>7</v>
+      <c r="M512" s="6">
+        <v>8</v>
       </c>
     </row>
     <row r="513" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A513" t="s">
         <v>50</v>
       </c>
+      <c r="B513" t="s">
+        <v>59</v>
+      </c>
       <c r="C513" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E513">
         <v>120</v>
@@ -19111,32 +19192,35 @@
       <c r="F513" s="3">
         <v>2</v>
       </c>
-      <c r="G513" s="7">
-        <v>18</v>
-      </c>
-      <c r="H513" s="7">
-        <v>5654</v>
-      </c>
-      <c r="I513" s="7">
-        <v>16776</v>
-      </c>
-      <c r="K513" s="7">
-        <v>188</v>
-      </c>
-      <c r="L513" s="7">
+      <c r="G513" s="6">
+        <v>23</v>
+      </c>
+      <c r="H513" s="6">
+        <v>7326</v>
+      </c>
+      <c r="I513" s="6">
+        <v>28223</v>
+      </c>
+      <c r="K513" s="6">
+        <v>230</v>
+      </c>
+      <c r="L513" s="6">
         <v>370</v>
       </c>
-      <c r="M513" s="7">
-        <v>8</v>
+      <c r="M513" s="6">
+        <v>10</v>
       </c>
     </row>
     <row r="514" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A514" t="s">
         <v>50</v>
       </c>
+      <c r="B514" t="s">
+        <v>59</v>
+      </c>
       <c r="C514" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E514">
         <v>120</v>
@@ -19144,32 +19228,35 @@
       <c r="F514" s="3">
         <v>2</v>
       </c>
-      <c r="G514" s="7">
-        <v>23</v>
-      </c>
-      <c r="H514" s="7">
-        <v>7326</v>
-      </c>
-      <c r="I514" s="7">
-        <v>28223</v>
-      </c>
-      <c r="K514" s="7">
-        <v>230</v>
-      </c>
-      <c r="L514" s="7">
-        <v>370</v>
-      </c>
-      <c r="M514" s="7">
-        <v>10</v>
+      <c r="G514" s="6">
+        <v>28</v>
+      </c>
+      <c r="H514" s="6">
+        <v>8488</v>
+      </c>
+      <c r="I514" s="6">
+        <v>39701</v>
+      </c>
+      <c r="K514" s="6">
+        <v>263</v>
+      </c>
+      <c r="L514" s="6">
+        <v>344</v>
+      </c>
+      <c r="M514" s="6">
+        <v>12</v>
       </c>
     </row>
     <row r="515" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A515" t="s">
         <v>50</v>
       </c>
+      <c r="B515" t="s">
+        <v>59</v>
+      </c>
       <c r="C515" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E515">
         <v>120</v>
@@ -19177,32 +19264,35 @@
       <c r="F515" s="3">
         <v>2</v>
       </c>
-      <c r="G515" s="7">
-        <v>28</v>
-      </c>
-      <c r="H515" s="7">
-        <v>8488</v>
-      </c>
-      <c r="I515" s="7">
-        <v>39701</v>
-      </c>
-      <c r="K515" s="7">
-        <v>263</v>
-      </c>
-      <c r="L515" s="7">
-        <v>344</v>
-      </c>
-      <c r="M515" s="7">
-        <v>12</v>
+      <c r="G515" s="6">
+        <v>33</v>
+      </c>
+      <c r="H515" s="6">
+        <v>9235</v>
+      </c>
+      <c r="I515" s="6">
+        <v>49816</v>
+      </c>
+      <c r="K515" s="6">
+        <v>286</v>
+      </c>
+      <c r="L515" s="6">
+        <v>295</v>
+      </c>
+      <c r="M515" s="6">
+        <v>13</v>
       </c>
     </row>
     <row r="516" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A516" t="s">
         <v>50</v>
       </c>
+      <c r="B516" t="s">
+        <v>59</v>
+      </c>
       <c r="C516" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
+        <v>SMC_2016_i+ii_SI50_120</v>
       </c>
       <c r="E516">
         <v>120</v>
@@ -19210,56 +19300,1211 @@
       <c r="F516" s="3">
         <v>2</v>
       </c>
-      <c r="G516" s="7">
-        <v>33</v>
-      </c>
-      <c r="H516" s="7">
-        <v>9235</v>
-      </c>
-      <c r="I516" s="7">
-        <v>49816</v>
-      </c>
-      <c r="K516" s="7">
-        <v>286</v>
-      </c>
-      <c r="L516" s="7">
-        <v>295</v>
-      </c>
-      <c r="M516" s="7">
-        <v>13</v>
+      <c r="G516" s="6">
+        <v>38</v>
+      </c>
+      <c r="H516" s="6">
+        <v>9695</v>
+      </c>
+      <c r="I516" s="6">
+        <v>58013</v>
+      </c>
+      <c r="K516" s="6">
+        <v>303</v>
+      </c>
+      <c r="L516" s="6">
+        <v>257</v>
+      </c>
+      <c r="M516" s="6">
+        <v>15</v>
       </c>
     </row>
     <row r="517" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A517" t="s">
         <v>50</v>
       </c>
+      <c r="B517" t="s">
+        <v>60</v>
+      </c>
       <c r="C517" t="str">
         <f t="shared" si="17"/>
-        <v>SMC_2016_SI50_120</v>
-      </c>
-      <c r="E517">
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E517" s="3">
+        <v>106</v>
+      </c>
+      <c r="F517" s="3">
+        <v>3</v>
+      </c>
+      <c r="G517" s="3">
+        <v>0</v>
+      </c>
+      <c r="H517" s="3">
+        <v>0</v>
+      </c>
+      <c r="I517" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="518" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A518" t="s">
+        <v>50</v>
+      </c>
+      <c r="B518" t="s">
+        <v>60</v>
+      </c>
+      <c r="C518" t="str">
+        <f t="shared" ref="C518:C560" si="18">IF(ISBLANK(B518),A518,A518&amp;"_"&amp;B518)&amp;IF(ISBLANK(D518),"_SI50_"&amp;E518,"_SI100_"&amp;D518)</f>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E518" s="3">
+        <v>106</v>
+      </c>
+      <c r="F518" s="3">
+        <v>3</v>
+      </c>
+      <c r="G518" s="3">
+        <v>5</v>
+      </c>
+      <c r="H518" s="3">
+        <v>0</v>
+      </c>
+      <c r="I518" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="519" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A519" t="s">
+        <v>50</v>
+      </c>
+      <c r="B519" t="s">
+        <v>60</v>
+      </c>
+      <c r="C519" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E519" s="3">
+        <v>106</v>
+      </c>
+      <c r="F519" s="3">
+        <v>3</v>
+      </c>
+      <c r="G519" s="3">
+        <v>10</v>
+      </c>
+      <c r="H519" s="3">
+        <v>45</v>
+      </c>
+      <c r="I519" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="520" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A520" t="s">
+        <v>50</v>
+      </c>
+      <c r="B520" t="s">
+        <v>60</v>
+      </c>
+      <c r="C520" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E520" s="3">
+        <v>106</v>
+      </c>
+      <c r="F520" s="3">
+        <v>3</v>
+      </c>
+      <c r="G520" s="3">
+        <v>15</v>
+      </c>
+      <c r="H520" s="3">
+        <v>396</v>
+      </c>
+      <c r="I520" s="3">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="521" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A521" t="s">
+        <v>50</v>
+      </c>
+      <c r="B521" t="s">
+        <v>60</v>
+      </c>
+      <c r="C521" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E521" s="3">
+        <v>106</v>
+      </c>
+      <c r="F521" s="3">
+        <v>3</v>
+      </c>
+      <c r="G521" s="3">
+        <v>20</v>
+      </c>
+      <c r="H521" s="3">
+        <v>1299</v>
+      </c>
+      <c r="I521" s="3">
+        <v>2499</v>
+      </c>
+    </row>
+    <row r="522" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A522" t="s">
+        <v>50</v>
+      </c>
+      <c r="B522" t="s">
+        <v>60</v>
+      </c>
+      <c r="C522" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E522" s="3">
+        <v>106</v>
+      </c>
+      <c r="F522" s="3">
+        <v>3</v>
+      </c>
+      <c r="G522" s="3">
+        <v>25</v>
+      </c>
+      <c r="H522" s="3">
+        <v>2613</v>
+      </c>
+      <c r="I522" s="3">
+        <v>7055</v>
+      </c>
+    </row>
+    <row r="523" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A523" t="s">
+        <v>50</v>
+      </c>
+      <c r="B523" t="s">
+        <v>60</v>
+      </c>
+      <c r="C523" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E523" s="3">
+        <v>106</v>
+      </c>
+      <c r="F523" s="3">
+        <v>3</v>
+      </c>
+      <c r="G523" s="3">
+        <v>30</v>
+      </c>
+      <c r="H523" s="3">
+        <v>4009</v>
+      </c>
+      <c r="I523" s="3">
+        <v>14213</v>
+      </c>
+    </row>
+    <row r="524" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A524" t="s">
+        <v>50</v>
+      </c>
+      <c r="B524" t="s">
+        <v>60</v>
+      </c>
+      <c r="C524" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E524" s="3">
+        <v>106</v>
+      </c>
+      <c r="F524" s="3">
+        <v>3</v>
+      </c>
+      <c r="G524" s="3">
+        <v>35</v>
+      </c>
+      <c r="H524" s="3">
+        <v>5241</v>
+      </c>
+      <c r="I524" s="3">
+        <v>23104</v>
+      </c>
+    </row>
+    <row r="525" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A525" t="s">
+        <v>50</v>
+      </c>
+      <c r="B525" t="s">
+        <v>60</v>
+      </c>
+      <c r="C525" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E525" s="3">
+        <v>106</v>
+      </c>
+      <c r="F525" s="3">
+        <v>3</v>
+      </c>
+      <c r="G525" s="3">
+        <v>40</v>
+      </c>
+      <c r="H525" s="3">
+        <v>6212</v>
+      </c>
+      <c r="I525" s="3">
+        <v>32560</v>
+      </c>
+    </row>
+    <row r="526" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A526" t="s">
+        <v>50</v>
+      </c>
+      <c r="B526" t="s">
+        <v>60</v>
+      </c>
+      <c r="C526" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E526" s="3">
+        <v>106</v>
+      </c>
+      <c r="F526" s="3">
+        <v>3</v>
+      </c>
+      <c r="G526" s="3">
+        <v>45</v>
+      </c>
+      <c r="H526" s="3">
+        <v>6926</v>
+      </c>
+      <c r="I526" s="3">
+        <v>41609</v>
+      </c>
+    </row>
+    <row r="527" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A527" t="s">
+        <v>50</v>
+      </c>
+      <c r="B527" t="s">
+        <v>60</v>
+      </c>
+      <c r="C527" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_106</v>
+      </c>
+      <c r="E527" s="3">
+        <v>106</v>
+      </c>
+      <c r="F527" s="3">
+        <v>3</v>
+      </c>
+      <c r="G527" s="3">
+        <v>50</v>
+      </c>
+      <c r="H527" s="3">
+        <v>7428</v>
+      </c>
+      <c r="I527" s="3">
+        <v>49651</v>
+      </c>
+    </row>
+    <row r="528" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A528" t="s">
+        <v>50</v>
+      </c>
+      <c r="B528" t="s">
+        <v>60</v>
+      </c>
+      <c r="C528" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E528" s="3">
+        <v>110</v>
+      </c>
+      <c r="F528" s="3">
+        <v>3</v>
+      </c>
+      <c r="G528" s="3">
+        <v>0</v>
+      </c>
+      <c r="H528" s="3">
+        <v>0</v>
+      </c>
+      <c r="I528" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="529" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A529" t="s">
+        <v>50</v>
+      </c>
+      <c r="B529" t="s">
+        <v>60</v>
+      </c>
+      <c r="C529" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E529" s="3">
+        <v>110</v>
+      </c>
+      <c r="F529" s="3">
+        <v>3</v>
+      </c>
+      <c r="G529" s="3">
+        <v>5</v>
+      </c>
+      <c r="H529" s="3">
+        <v>0</v>
+      </c>
+      <c r="I529" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="530" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A530" t="s">
+        <v>50</v>
+      </c>
+      <c r="B530" t="s">
+        <v>60</v>
+      </c>
+      <c r="C530" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E530" s="3">
+        <v>110</v>
+      </c>
+      <c r="F530" s="3">
+        <v>3</v>
+      </c>
+      <c r="G530" s="3">
+        <v>10</v>
+      </c>
+      <c r="H530" s="3">
+        <v>52</v>
+      </c>
+      <c r="I530" s="3">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="531" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A531" t="s">
+        <v>50</v>
+      </c>
+      <c r="B531" t="s">
+        <v>60</v>
+      </c>
+      <c r="C531" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E531" s="3">
+        <v>110</v>
+      </c>
+      <c r="F531" s="3">
+        <v>3</v>
+      </c>
+      <c r="G531" s="3">
+        <v>15</v>
+      </c>
+      <c r="H531" s="3">
+        <v>452</v>
+      </c>
+      <c r="I531" s="3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="532" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A532" t="s">
+        <v>50</v>
+      </c>
+      <c r="B532" t="s">
+        <v>60</v>
+      </c>
+      <c r="C532" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E532" s="3">
+        <v>110</v>
+      </c>
+      <c r="F532" s="3">
+        <v>3</v>
+      </c>
+      <c r="G532" s="3">
+        <v>20</v>
+      </c>
+      <c r="H532" s="3">
+        <v>1463</v>
+      </c>
+      <c r="I532" s="3">
+        <v>2900</v>
+      </c>
+    </row>
+    <row r="533" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A533" t="s">
+        <v>50</v>
+      </c>
+      <c r="B533" t="s">
+        <v>60</v>
+      </c>
+      <c r="C533" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E533" s="3">
+        <v>110</v>
+      </c>
+      <c r="F533" s="3">
+        <v>3</v>
+      </c>
+      <c r="G533" s="3">
+        <v>25</v>
+      </c>
+      <c r="H533" s="3">
+        <v>2914</v>
+      </c>
+      <c r="I533" s="3">
+        <v>7978</v>
+      </c>
+    </row>
+    <row r="534" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A534" t="s">
+        <v>50</v>
+      </c>
+      <c r="B534" t="s">
+        <v>60</v>
+      </c>
+      <c r="C534" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E534" s="3">
+        <v>110</v>
+      </c>
+      <c r="F534" s="3">
+        <v>3</v>
+      </c>
+      <c r="G534" s="3">
+        <v>30</v>
+      </c>
+      <c r="H534" s="3">
+        <v>4436</v>
+      </c>
+      <c r="I534" s="3">
+        <v>15722</v>
+      </c>
+    </row>
+    <row r="535" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A535" t="s">
+        <v>50</v>
+      </c>
+      <c r="B535" t="s">
+        <v>60</v>
+      </c>
+      <c r="C535" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E535" s="3">
+        <v>110</v>
+      </c>
+      <c r="F535" s="3">
+        <v>3</v>
+      </c>
+      <c r="G535" s="3">
+        <v>35</v>
+      </c>
+      <c r="H535" s="3">
+        <v>5764</v>
+      </c>
+      <c r="I535" s="3">
+        <v>25084</v>
+      </c>
+    </row>
+    <row r="536" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A536" t="s">
+        <v>50</v>
+      </c>
+      <c r="B536" t="s">
+        <v>60</v>
+      </c>
+      <c r="C536" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E536" s="3">
+        <v>110</v>
+      </c>
+      <c r="F536" s="3">
+        <v>3</v>
+      </c>
+      <c r="G536" s="3">
+        <v>40</v>
+      </c>
+      <c r="H536" s="3">
+        <v>6801</v>
+      </c>
+      <c r="I536" s="3">
+        <v>34802</v>
+      </c>
+    </row>
+    <row r="537" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A537" t="s">
+        <v>50</v>
+      </c>
+      <c r="B537" t="s">
+        <v>60</v>
+      </c>
+      <c r="C537" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E537" s="3">
+        <v>110</v>
+      </c>
+      <c r="F537" s="3">
+        <v>3</v>
+      </c>
+      <c r="G537" s="3">
+        <v>45</v>
+      </c>
+      <c r="H537" s="3">
+        <v>7557</v>
+      </c>
+      <c r="I537" s="3">
+        <v>43899</v>
+      </c>
+    </row>
+    <row r="538" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A538" t="s">
+        <v>50</v>
+      </c>
+      <c r="B538" t="s">
+        <v>60</v>
+      </c>
+      <c r="C538" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_110</v>
+      </c>
+      <c r="E538" s="3">
+        <v>110</v>
+      </c>
+      <c r="F538" s="3">
+        <v>3</v>
+      </c>
+      <c r="G538" s="3">
+        <v>50</v>
+      </c>
+      <c r="H538" s="3">
+        <v>8084</v>
+      </c>
+      <c r="I538" s="3">
+        <v>51827</v>
+      </c>
+    </row>
+    <row r="539" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A539" t="s">
+        <v>50</v>
+      </c>
+      <c r="B539" t="s">
+        <v>60</v>
+      </c>
+      <c r="C539" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E539" s="3">
+        <v>115</v>
+      </c>
+      <c r="F539" s="3">
+        <v>2</v>
+      </c>
+      <c r="G539" s="3">
+        <v>0</v>
+      </c>
+      <c r="H539" s="3">
+        <v>0</v>
+      </c>
+      <c r="I539" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="540" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A540" t="s">
+        <v>50</v>
+      </c>
+      <c r="B540" t="s">
+        <v>60</v>
+      </c>
+      <c r="C540" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E540" s="3">
+        <v>115</v>
+      </c>
+      <c r="F540" s="3">
+        <v>2</v>
+      </c>
+      <c r="G540" s="3">
+        <v>5</v>
+      </c>
+      <c r="H540" s="3">
+        <v>1</v>
+      </c>
+      <c r="I540" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="541" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A541" t="s">
+        <v>50</v>
+      </c>
+      <c r="B541" t="s">
+        <v>60</v>
+      </c>
+      <c r="C541" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E541" s="3">
+        <v>115</v>
+      </c>
+      <c r="F541" s="3">
+        <v>2</v>
+      </c>
+      <c r="G541" s="3">
+        <v>10</v>
+      </c>
+      <c r="H541" s="3">
+        <v>63</v>
+      </c>
+      <c r="I541" s="3">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="542" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A542" t="s">
+        <v>50</v>
+      </c>
+      <c r="B542" t="s">
+        <v>60</v>
+      </c>
+      <c r="C542" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E542" s="3">
+        <v>115</v>
+      </c>
+      <c r="F542" s="3">
+        <v>2</v>
+      </c>
+      <c r="G542" s="3">
+        <v>15</v>
+      </c>
+      <c r="H542" s="3">
+        <v>536</v>
+      </c>
+      <c r="I542" s="3">
+        <v>749</v>
+      </c>
+    </row>
+    <row r="543" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A543" t="s">
+        <v>50</v>
+      </c>
+      <c r="B543" t="s">
+        <v>60</v>
+      </c>
+      <c r="C543" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E543" s="3">
+        <v>115</v>
+      </c>
+      <c r="F543" s="3">
+        <v>2</v>
+      </c>
+      <c r="G543" s="3">
+        <v>20</v>
+      </c>
+      <c r="H543" s="3">
+        <v>1708</v>
+      </c>
+      <c r="I543" s="3">
+        <v>3495</v>
+      </c>
+    </row>
+    <row r="544" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A544" t="s">
+        <v>50</v>
+      </c>
+      <c r="B544" t="s">
+        <v>60</v>
+      </c>
+      <c r="C544" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E544" s="3">
+        <v>115</v>
+      </c>
+      <c r="F544" s="3">
+        <v>2</v>
+      </c>
+      <c r="G544" s="3">
+        <v>25</v>
+      </c>
+      <c r="H544" s="3">
+        <v>3357</v>
+      </c>
+      <c r="I544" s="3">
+        <v>9299</v>
+      </c>
+    </row>
+    <row r="545" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A545" t="s">
+        <v>50</v>
+      </c>
+      <c r="B545" t="s">
+        <v>60</v>
+      </c>
+      <c r="C545" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E545" s="3">
+        <v>115</v>
+      </c>
+      <c r="F545" s="3">
+        <v>2</v>
+      </c>
+      <c r="G545" s="3">
+        <v>30</v>
+      </c>
+      <c r="H545" s="3">
+        <v>5057</v>
+      </c>
+      <c r="I545" s="3">
+        <v>17810</v>
+      </c>
+    </row>
+    <row r="546" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A546" t="s">
+        <v>50</v>
+      </c>
+      <c r="B546" t="s">
+        <v>60</v>
+      </c>
+      <c r="C546" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E546" s="3">
+        <v>115</v>
+      </c>
+      <c r="F546" s="3">
+        <v>2</v>
+      </c>
+      <c r="G546" s="3">
+        <v>35</v>
+      </c>
+      <c r="H546" s="3">
+        <v>6520</v>
+      </c>
+      <c r="I546" s="3">
+        <v>27743</v>
+      </c>
+    </row>
+    <row r="547" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A547" t="s">
+        <v>50</v>
+      </c>
+      <c r="B547" t="s">
+        <v>60</v>
+      </c>
+      <c r="C547" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E547" s="3">
+        <v>115</v>
+      </c>
+      <c r="F547" s="3">
+        <v>2</v>
+      </c>
+      <c r="G547" s="3">
+        <v>40</v>
+      </c>
+      <c r="H547" s="3">
+        <v>7648</v>
+      </c>
+      <c r="I547" s="3">
+        <v>37733</v>
+      </c>
+    </row>
+    <row r="548" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A548" t="s">
+        <v>50</v>
+      </c>
+      <c r="B548" t="s">
+        <v>60</v>
+      </c>
+      <c r="C548" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E548" s="3">
+        <v>115</v>
+      </c>
+      <c r="F548" s="3">
+        <v>2</v>
+      </c>
+      <c r="G548" s="3">
+        <v>45</v>
+      </c>
+      <c r="H548" s="3">
+        <v>8460</v>
+      </c>
+      <c r="I548" s="3">
+        <v>46823</v>
+      </c>
+    </row>
+    <row r="549" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A549" t="s">
+        <v>50</v>
+      </c>
+      <c r="B549" t="s">
+        <v>60</v>
+      </c>
+      <c r="C549" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_115</v>
+      </c>
+      <c r="E549" s="3">
+        <v>115</v>
+      </c>
+      <c r="F549" s="3">
+        <v>2</v>
+      </c>
+      <c r="G549" s="3">
+        <v>50</v>
+      </c>
+      <c r="H549" s="3">
+        <v>9022</v>
+      </c>
+      <c r="I549" s="3">
+        <v>54545</v>
+      </c>
+    </row>
+    <row r="550" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A550" t="s">
+        <v>50</v>
+      </c>
+      <c r="B550" t="s">
+        <v>60</v>
+      </c>
+      <c r="C550" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E550" s="3">
         <v>120</v>
       </c>
-      <c r="F517" s="3">
+      <c r="F550" s="3">
         <v>2</v>
       </c>
-      <c r="G517" s="7">
-        <v>38</v>
-      </c>
-      <c r="H517" s="7">
-        <v>9695</v>
-      </c>
-      <c r="I517" s="7">
-        <v>58013</v>
-      </c>
-      <c r="K517" s="7">
-        <v>303</v>
-      </c>
-      <c r="L517" s="7">
-        <v>257</v>
-      </c>
-      <c r="M517" s="7">
+      <c r="G550" s="3">
+        <v>0</v>
+      </c>
+      <c r="H550" s="3">
+        <v>0</v>
+      </c>
+      <c r="I550" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="551" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A551" t="s">
+        <v>50</v>
+      </c>
+      <c r="B551" t="s">
+        <v>60</v>
+      </c>
+      <c r="C551" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E551" s="3">
+        <v>120</v>
+      </c>
+      <c r="F551" s="3">
+        <v>2</v>
+      </c>
+      <c r="G551" s="3">
+        <v>5</v>
+      </c>
+      <c r="H551" s="3">
+        <v>1</v>
+      </c>
+      <c r="I551" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="552" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A552" t="s">
+        <v>50</v>
+      </c>
+      <c r="B552" t="s">
+        <v>60</v>
+      </c>
+      <c r="C552" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E552" s="3">
+        <v>120</v>
+      </c>
+      <c r="F552" s="3">
+        <v>2</v>
+      </c>
+      <c r="G552" s="3">
+        <v>10</v>
+      </c>
+      <c r="H552" s="3">
+        <v>76</v>
+      </c>
+      <c r="I552" s="3">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="553" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A553" t="s">
+        <v>50</v>
+      </c>
+      <c r="B553" t="s">
+        <v>60</v>
+      </c>
+      <c r="C553" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E553" s="3">
+        <v>120</v>
+      </c>
+      <c r="F553" s="3">
+        <v>2</v>
+      </c>
+      <c r="G553" s="3">
         <v>15</v>
+      </c>
+      <c r="H553" s="3">
+        <v>633</v>
+      </c>
+      <c r="I553" s="3">
+        <v>927</v>
+      </c>
+    </row>
+    <row r="554" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A554" t="s">
+        <v>50</v>
+      </c>
+      <c r="B554" t="s">
+        <v>60</v>
+      </c>
+      <c r="C554" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E554" s="3">
+        <v>120</v>
+      </c>
+      <c r="F554" s="3">
+        <v>2</v>
+      </c>
+      <c r="G554" s="3">
+        <v>20</v>
+      </c>
+      <c r="H554" s="3">
+        <v>1983</v>
+      </c>
+      <c r="I554" s="3">
+        <v>4163</v>
+      </c>
+    </row>
+    <row r="555" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A555" t="s">
+        <v>50</v>
+      </c>
+      <c r="B555" t="s">
+        <v>60</v>
+      </c>
+      <c r="C555" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E555" s="3">
+        <v>120</v>
+      </c>
+      <c r="F555" s="3">
+        <v>2</v>
+      </c>
+      <c r="G555" s="3">
+        <v>25</v>
+      </c>
+      <c r="H555" s="3">
+        <v>3847</v>
+      </c>
+      <c r="I555" s="3">
+        <v>10718</v>
+      </c>
+    </row>
+    <row r="556" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A556" t="s">
+        <v>50</v>
+      </c>
+      <c r="B556" t="s">
+        <v>60</v>
+      </c>
+      <c r="C556" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E556" s="3">
+        <v>120</v>
+      </c>
+      <c r="F556" s="3">
+        <v>2</v>
+      </c>
+      <c r="G556" s="3">
+        <v>30</v>
+      </c>
+      <c r="H556" s="3">
+        <v>5738</v>
+      </c>
+      <c r="I556" s="3">
+        <v>19969</v>
+      </c>
+    </row>
+    <row r="557" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A557" t="s">
+        <v>50</v>
+      </c>
+      <c r="B557" t="s">
+        <v>60</v>
+      </c>
+      <c r="C557" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E557" s="3">
+        <v>120</v>
+      </c>
+      <c r="F557" s="3">
+        <v>2</v>
+      </c>
+      <c r="G557" s="3">
+        <v>35</v>
+      </c>
+      <c r="H557" s="3">
+        <v>7341</v>
+      </c>
+      <c r="I557" s="3">
+        <v>30403</v>
+      </c>
+    </row>
+    <row r="558" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A558" t="s">
+        <v>50</v>
+      </c>
+      <c r="B558" t="s">
+        <v>60</v>
+      </c>
+      <c r="C558" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E558" s="3">
+        <v>120</v>
+      </c>
+      <c r="F558" s="3">
+        <v>2</v>
+      </c>
+      <c r="G558" s="3">
+        <v>40</v>
+      </c>
+      <c r="H558" s="3">
+        <v>8562</v>
+      </c>
+      <c r="I558" s="3">
+        <v>40579</v>
+      </c>
+    </row>
+    <row r="559" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A559" t="s">
+        <v>50</v>
+      </c>
+      <c r="B559" t="s">
+        <v>60</v>
+      </c>
+      <c r="C559" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E559" s="3">
+        <v>120</v>
+      </c>
+      <c r="F559" s="3">
+        <v>2</v>
+      </c>
+      <c r="G559" s="3">
+        <v>45</v>
+      </c>
+      <c r="H559" s="3">
+        <v>9432</v>
+      </c>
+      <c r="I559" s="3">
+        <v>49588</v>
+      </c>
+    </row>
+    <row r="560" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A560" t="s">
+        <v>50</v>
+      </c>
+      <c r="B560" t="s">
+        <v>60</v>
+      </c>
+      <c r="C560" t="str">
+        <f t="shared" si="18"/>
+        <v>SMC_2016_i+ii+iii_SI50_120</v>
+      </c>
+      <c r="E560" s="3">
+        <v>120</v>
+      </c>
+      <c r="F560" s="3">
+        <v>2</v>
+      </c>
+      <c r="G560" s="3">
+        <v>50</v>
+      </c>
+      <c r="H560" s="3">
+        <v>10028</v>
+      </c>
+      <c r="I560" s="3">
+        <v>57056</v>
       </c>
     </row>
   </sheetData>

</xml_diff>